<commit_message>
test-22: 2Y + extrapol
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-22.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-22.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
   <si>
     <t>Random Forest-100 (superdataset-24-f 3Ysum.csv)</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>RF-100 (superdataset-24-f 3Y.csv + extrapol)</t>
+  </si>
+  <si>
+    <t>RF-100 (superdataset-24-f 2Y.csv + extrapol)</t>
   </si>
 </sst>
 </file>
@@ -1361,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:T67"/>
+  <dimension ref="C3:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="X47" sqref="X47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U71" sqref="U71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1376,7 @@
     <col min="8" max="8" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1387,10 +1390,13 @@
       </c>
       <c r="P3" s="1"/>
       <c r="S3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>1</v>
@@ -1413,8 +1419,12 @@
       <c r="T4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -1444,10 +1454,16 @@
         <v>1</v>
       </c>
       <c r="T5" s="3">
+        <v>0.74759938062002673</v>
+      </c>
+      <c r="X5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="3">
         <v>0.71804558825725728</v>
       </c>
     </row>
-    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -1481,10 +1497,17 @@
         <v>2</v>
       </c>
       <c r="T6" s="3">
+        <v>0.75272216793297142</v>
+      </c>
+      <c r="X6" s="2">
+        <f>X5+1</f>
+        <v>2</v>
+      </c>
+      <c r="Y6" s="3">
         <v>0.72185381859637232</v>
       </c>
     </row>
-    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -1518,10 +1541,17 @@
         <v>3</v>
       </c>
       <c r="T7" s="3">
+        <v>0.81290062745285052</v>
+      </c>
+      <c r="X7" s="2">
+        <f t="shared" ref="X7:X54" si="4">X6+1</f>
+        <v>3</v>
+      </c>
+      <c r="Y7" s="3">
         <v>0.6981084741413246</v>
       </c>
     </row>
-    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1555,10 +1585,17 @@
         <v>4</v>
       </c>
       <c r="T8" s="3">
+        <v>0.76359659281275505</v>
+      </c>
+      <c r="X8" s="2">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="Y8" s="3">
         <v>0.71829244406514348</v>
       </c>
     </row>
-    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1592,10 +1629,17 @@
         <v>5</v>
       </c>
       <c r="T9" s="3">
+        <v>0.7545887963884832</v>
+      </c>
+      <c r="X9" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="Y9" s="3">
         <v>0.65047079592362311</v>
       </c>
     </row>
-    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1629,10 +1673,17 @@
         <v>6</v>
       </c>
       <c r="T10" s="3">
+        <v>0.80385166737402391</v>
+      </c>
+      <c r="X10" s="2">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="Y10" s="3">
         <v>0.63502855952427495</v>
       </c>
     </row>
-    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1666,10 +1717,17 @@
         <v>7</v>
       </c>
       <c r="T11" s="3">
+        <v>0.81537059224632424</v>
+      </c>
+      <c r="X11" s="2">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="Y11" s="3">
         <v>0.713213169608098</v>
       </c>
     </row>
-    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1703,10 +1761,17 @@
         <v>8</v>
       </c>
       <c r="T12" s="3">
+        <v>0.80425470934478516</v>
+      </c>
+      <c r="X12" s="2">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="Y12" s="3">
         <v>0.69011361740712807</v>
       </c>
     </row>
-    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1740,10 +1805,17 @@
         <v>9</v>
       </c>
       <c r="T13" s="3">
+        <v>0.7576941490745841</v>
+      </c>
+      <c r="X13" s="2">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="Y13" s="3">
         <v>0.70561048728582532</v>
       </c>
     </row>
-    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1777,10 +1849,17 @@
         <v>10</v>
       </c>
       <c r="T14" s="3">
+        <v>0.74667295040812309</v>
+      </c>
+      <c r="X14" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="Y14" s="3">
         <v>0.66811210736681925</v>
       </c>
     </row>
-    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1814,10 +1893,17 @@
         <v>11</v>
       </c>
       <c r="T15" s="3">
+        <v>0.78479006333818369</v>
+      </c>
+      <c r="X15" s="2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="Y15" s="3">
         <v>0.68557594968839686</v>
       </c>
     </row>
-    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1851,10 +1937,17 @@
         <v>12</v>
       </c>
       <c r="T16" s="3">
+        <v>0.77498508287134604</v>
+      </c>
+      <c r="X16" s="2">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="Y16" s="3">
         <v>0.6851485124334683</v>
       </c>
     </row>
-    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1888,10 +1981,17 @@
         <v>13</v>
       </c>
       <c r="T17" s="3">
+        <v>0.76680506361277445</v>
+      </c>
+      <c r="X17" s="2">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="Y17" s="3">
         <v>0.62803686401783998</v>
       </c>
     </row>
-    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1925,10 +2025,17 @@
         <v>14</v>
       </c>
       <c r="T18" s="3">
+        <v>0.79547860900348266</v>
+      </c>
+      <c r="X18" s="2">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="Y18" s="3">
         <v>0.69475380219944394</v>
       </c>
     </row>
-    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1962,10 +2069,17 @@
         <v>15</v>
       </c>
       <c r="T19" s="3">
+        <v>0.80253923797160254</v>
+      </c>
+      <c r="X19" s="2">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="Y19" s="3">
         <v>0.66275212975079434</v>
       </c>
     </row>
-    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1999,10 +2113,17 @@
         <v>16</v>
       </c>
       <c r="T20" s="3">
+        <v>0.75811037408550375</v>
+      </c>
+      <c r="X20" s="2">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="Y20" s="3">
         <v>0.66840503818741026</v>
       </c>
     </row>
-    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2036,10 +2157,17 @@
         <v>17</v>
       </c>
       <c r="T21" s="3">
+        <v>0.80959496508752071</v>
+      </c>
+      <c r="X21" s="2">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="Y21" s="3">
         <v>0.64333505103013144</v>
       </c>
     </row>
-    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2073,10 +2201,17 @@
         <v>18</v>
       </c>
       <c r="T22" s="3">
+        <v>0.78243223145681651</v>
+      </c>
+      <c r="X22" s="2">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="Y22" s="3">
         <v>0.69545562366911273</v>
       </c>
     </row>
-    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2110,10 +2245,17 @@
         <v>19</v>
       </c>
       <c r="T23" s="3">
+        <v>0.79065531295771696</v>
+      </c>
+      <c r="X23" s="2">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="Y23" s="3">
         <v>0.68440236121772313</v>
       </c>
     </row>
-    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2147,10 +2289,17 @@
         <v>20</v>
       </c>
       <c r="T24" s="3">
+        <v>0.75111177334431645</v>
+      </c>
+      <c r="X24" s="2">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="Y24" s="3">
         <v>0.66391507977526842</v>
       </c>
     </row>
-    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2184,10 +2333,17 @@
         <v>21</v>
       </c>
       <c r="T25" s="3">
+        <v>0.7933349338637159</v>
+      </c>
+      <c r="X25" s="2">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="Y25" s="3">
         <v>0.66425350778334002</v>
       </c>
     </row>
-    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2221,10 +2377,17 @@
         <v>22</v>
       </c>
       <c r="T26" s="3">
+        <v>0.7431987341233699</v>
+      </c>
+      <c r="X26" s="2">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="Y26" s="3">
         <v>0.718111569087034</v>
       </c>
     </row>
-    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2258,10 +2421,17 @@
         <v>23</v>
       </c>
       <c r="T27" s="3">
+        <v>0.80481897041530459</v>
+      </c>
+      <c r="X27" s="2">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="Y27" s="3">
         <v>0.58926158900661996</v>
       </c>
     </row>
-    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2295,10 +2465,17 @@
         <v>24</v>
       </c>
       <c r="T28" s="3">
+        <v>0.77831347161363618</v>
+      </c>
+      <c r="X28" s="2">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="Y28" s="3">
         <v>0.6880634305504858</v>
       </c>
     </row>
-    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2332,10 +2509,17 @@
         <v>25</v>
       </c>
       <c r="T29" s="3">
+        <v>0.73250447421016152</v>
+      </c>
+      <c r="X29" s="2">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="Y29" s="3">
         <v>0.66240162760884957</v>
       </c>
     </row>
-    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2369,10 +2553,17 @@
         <v>26</v>
       </c>
       <c r="T30" s="3">
+        <v>0.79928969776231029</v>
+      </c>
+      <c r="X30" s="2">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="Y30" s="3">
         <v>0.62962520878089356</v>
       </c>
     </row>
-    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2406,10 +2597,17 @@
         <v>27</v>
       </c>
       <c r="T31" s="3">
+        <v>0.80145040301035131</v>
+      </c>
+      <c r="X31" s="2">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="Y31" s="3">
         <v>0.70429496117698243</v>
       </c>
     </row>
-    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2443,10 +2641,17 @@
         <v>28</v>
       </c>
       <c r="T32" s="3">
+        <v>0.79203197789581958</v>
+      </c>
+      <c r="X32" s="2">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="Y32" s="3">
         <v>0.73460558179431357</v>
       </c>
     </row>
-    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2480,10 +2685,17 @@
         <v>29</v>
       </c>
       <c r="T33" s="3">
+        <v>0.74549347792987275</v>
+      </c>
+      <c r="X33" s="2">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="Y33" s="3">
         <v>0.6695388415189456</v>
       </c>
     </row>
-    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2517,10 +2729,17 @@
         <v>30</v>
       </c>
       <c r="T34" s="3">
+        <v>0.78356932624316888</v>
+      </c>
+      <c r="X34" s="2">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="Y34" s="3">
         <v>0.68027852618929274</v>
       </c>
     </row>
-    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2554,10 +2773,17 @@
         <v>31</v>
       </c>
       <c r="T35" s="3">
+        <v>0.78165766235738088</v>
+      </c>
+      <c r="X35" s="2">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="Y35" s="3">
         <v>0.6993139246063016</v>
       </c>
     </row>
-    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2591,10 +2817,17 @@
         <v>32</v>
       </c>
       <c r="T36" s="3">
+        <v>0.8129048890288546</v>
+      </c>
+      <c r="X36" s="2">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="Y36" s="3">
         <v>0.72318087625019356</v>
       </c>
     </row>
-    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2628,10 +2861,17 @@
         <v>33</v>
       </c>
       <c r="T37" s="3">
+        <v>0.80361307339161958</v>
+      </c>
+      <c r="X37" s="2">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="Y37" s="3">
         <v>0.67643500801796064</v>
       </c>
     </row>
-    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2665,10 +2905,17 @@
         <v>34</v>
       </c>
       <c r="T38" s="3">
+        <v>0.77850151482103791</v>
+      </c>
+      <c r="X38" s="2">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="Y38" s="3">
         <v>0.63680085907475925</v>
       </c>
     </row>
-    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2702,10 +2949,17 @@
         <v>35</v>
       </c>
       <c r="T39" s="3">
+        <v>0.76357957335404536</v>
+      </c>
+      <c r="X39" s="2">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="Y39" s="3">
         <v>0.75748717948567634</v>
       </c>
     </row>
-    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2739,10 +2993,17 @@
         <v>36</v>
       </c>
       <c r="T40" s="3">
+        <v>0.82719591105098256</v>
+      </c>
+      <c r="X40" s="2">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="Y40" s="3">
         <v>0.6527747799660627</v>
       </c>
     </row>
-    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2776,10 +3037,17 @@
         <v>37</v>
       </c>
       <c r="T41" s="3">
+        <v>0.78768718630391255</v>
+      </c>
+      <c r="X41" s="2">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="Y41" s="3">
         <v>0.67055880848726712</v>
       </c>
     </row>
-    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2813,10 +3081,17 @@
         <v>38</v>
       </c>
       <c r="T42" s="3">
+        <v>0.80721891304325188</v>
+      </c>
+      <c r="X42" s="2">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="Y42" s="3">
         <v>0.62658464583364371</v>
       </c>
     </row>
-    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2850,10 +3125,17 @@
         <v>39</v>
       </c>
       <c r="T43" s="3">
+        <v>0.80684801694652231</v>
+      </c>
+      <c r="X43" s="2">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="Y43" s="3">
         <v>0.70583496249645283</v>
       </c>
     </row>
-    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2887,10 +3169,17 @@
         <v>40</v>
       </c>
       <c r="T44" s="3">
+        <v>0.77865927003954072</v>
+      </c>
+      <c r="X44" s="2">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="Y44" s="3">
         <v>0.65343318008461004</v>
       </c>
     </row>
-    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2924,10 +3213,17 @@
         <v>41</v>
       </c>
       <c r="T45" s="3">
+        <v>0.78440058195670237</v>
+      </c>
+      <c r="X45" s="2">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="Y45" s="3">
         <v>0.63720884986360993</v>
       </c>
     </row>
-    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2961,10 +3257,17 @@
         <v>42</v>
       </c>
       <c r="T46" s="3">
+        <v>0.77517757569569157</v>
+      </c>
+      <c r="X46" s="2">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="Y46" s="3">
         <v>0.7059213929907977</v>
       </c>
     </row>
-    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2998,10 +3301,17 @@
         <v>43</v>
       </c>
       <c r="T47" s="3">
+        <v>0.73172178530723397</v>
+      </c>
+      <c r="X47" s="2">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="Y47" s="3">
         <v>0.62604470493530884</v>
       </c>
     </row>
-    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3035,10 +3345,17 @@
         <v>44</v>
       </c>
       <c r="T48" s="3">
+        <v>0.78739711178736771</v>
+      </c>
+      <c r="X48" s="2">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="Y48" s="3">
         <v>0.66627333730157168</v>
       </c>
     </row>
-    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3072,10 +3389,17 @@
         <v>45</v>
       </c>
       <c r="T49" s="3">
+        <v>0.76981245439444945</v>
+      </c>
+      <c r="X49" s="2">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="Y49" s="3">
         <v>0.66292406711079277</v>
       </c>
     </row>
-    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3109,10 +3433,17 @@
         <v>46</v>
       </c>
       <c r="T50" s="3">
+        <v>0.74310584214061914</v>
+      </c>
+      <c r="X50" s="2">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="Y50" s="3">
         <v>0.65075574089508481</v>
       </c>
     </row>
-    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3146,10 +3477,17 @@
         <v>47</v>
       </c>
       <c r="T51" s="3">
+        <v>0.80322037948211167</v>
+      </c>
+      <c r="X51" s="2">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="Y51" s="3">
         <v>0.70793932329002096</v>
       </c>
     </row>
-    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3183,10 +3521,17 @@
         <v>48</v>
       </c>
       <c r="T52" s="3">
+        <v>0.78192280972213579</v>
+      </c>
+      <c r="X52" s="2">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="Y52" s="3">
         <v>0.68647072570056089</v>
       </c>
     </row>
-    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -3220,10 +3565,17 @@
         <v>49</v>
       </c>
       <c r="T53" s="3">
+        <v>0.74027177131612953</v>
+      </c>
+      <c r="X53" s="2">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="Y53" s="3">
         <v>0.66932989478909277</v>
       </c>
     </row>
-    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3257,10 +3609,17 @@
         <v>50</v>
       </c>
       <c r="T54" s="3">
+        <v>0.77066450762997896</v>
+      </c>
+      <c r="X54" s="2">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="Y54" s="3">
         <v>0.72746954695321864</v>
       </c>
     </row>
-    <row r="56" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>3</v>
       </c>
@@ -3296,10 +3655,17 @@
       </c>
       <c r="T56" s="3">
         <f>AVERAGE(T5:T54)</f>
+        <v>0.77970641288442966</v>
+      </c>
+      <c r="X56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y56" s="3">
+        <f>AVERAGE(Y5:Y54)</f>
         <v>0.67827612251550418</v>
       </c>
     </row>
-    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>4</v>
       </c>
@@ -3335,6 +3701,13 @@
       </c>
       <c r="T57" s="3">
         <f>_xlfn.STDEV.S(T5:T54)</f>
+        <v>2.4509800244337382E-2</v>
+      </c>
+      <c r="X57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y57" s="3">
+        <f>_xlfn.STDEV.S(Y5:Y54)</f>
         <v>3.4003288288829397E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test 22: extra 2Y r2
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-22.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-22.xlsx
@@ -8,8 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="r2" sheetId="1" r:id="rId1"/>
-    <sheet name="mae" sheetId="2" r:id="rId2"/>
-    <sheet name="mse" sheetId="3" r:id="rId3"/>
+    <sheet name="r2 (2Ysum)" sheetId="4" r:id="rId2"/>
+    <sheet name="mae" sheetId="2" r:id="rId3"/>
+    <sheet name="mse" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="20">
   <si>
     <t>Random Forest-100 (superdataset-24-f 3Ysum.csv)</t>
   </si>
@@ -78,6 +79,9 @@
   </si>
   <si>
     <t>(third year * 3)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24-f 2Ysum.csv)</t>
   </si>
 </sst>
 </file>
@@ -918,7 +922,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1016,7 +1019,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3279,8 +3281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:Y67"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5671,9 +5673,1304 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:O57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.93150131168613637</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.48158352219436151</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.7328261160883589</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <f>C5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.92937188802588511</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.51374867566029625</v>
+      </c>
+      <c r="I6" s="2">
+        <f>I5+1</f>
+        <v>2</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.81156795793393999</v>
+      </c>
+      <c r="N6" s="2">
+        <f>N5+1</f>
+        <v>2</v>
+      </c>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:C54" si="0">C6+1</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.92816576041059184</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.53398838623476363</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" ref="I7:I54" si="1">I6+1</f>
+        <v>3</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.78895231922312026</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" ref="N7:N54" si="2">N6+1</f>
+        <v>3</v>
+      </c>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.93058878099651565</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.53561266794425677</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.83283066195875255</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.92994795806995567</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.45748876950753081</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.77883834797005469</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.92968496353074004</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.48381749646353017</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.76571336575083537</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.93042005938377392</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.53083944161761398</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.77190474471957016</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.93045742861543168</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.48766686221497091</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.74143615641260419</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.93153463278398718</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.50731254894258271</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.81948870997368461</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.93240175587189034</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.48798875019573951</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.77034405579522025</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.93366489105197503</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.49795235066818172</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.79758876088385089</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.93255159291706469</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.51559911271845593</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.76195408003286547</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.93065740591097657</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.50873136960700849</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.74964674834410983</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.93040957575384831</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.51909231727920913</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.75346932384082188</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.93143326530503567</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.48324327911865861</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.78668206422229736</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.9272634859141996</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.53677297537956636</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.75543843228912744</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.93081517984767637</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.54593808844202818</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.78173828401931256</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.93051178589247086</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.5126328686153625</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.7927907612647439</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.93151541924309023</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.50504173424329535</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0.7992002650369554</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.92967010106471115</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.54118422614498574</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0.79576976186300852</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.92949217784545068</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.52363980369992436</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0.75158070984674707</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.93035596633835738</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.47924862956313141</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0.7800408627700568</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.93099968399584432</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.52125520804731207</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0.77870660781914558</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.92754414634808358</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.49940020845842881</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.76174899013519481</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.93087809788640896</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.53843839502352986</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0.77091959415287703</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.93232568205862421</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.54402084820828944</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0.77427505679205644</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.92881601700134042</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.52084507191612883</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0.75058708408046437</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O31" s="3"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.92724674655940187</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.52333816497346608</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0.80091715014380749</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.929123089208296</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.48551896960273833</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0.79280340328115162</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.92688863937515098</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.49931852176302838</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0.73302701977319129</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O34" s="3"/>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.92841239488108818</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.5292294032568301</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0.76039576791459251</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O35" s="3"/>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.93032160985634504</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0.53820389859832418</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0.78802817783949064</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O36" s="3"/>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.93119936222312527</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0.50577583149120409</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0.81305402062467935</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O37" s="3"/>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.93191612289777748</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0.48600758598846161</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="J38" s="3">
+        <v>0.68953577597343774</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.93139810604088336</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0.53388510925371924</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0.81338973318411723</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="O39" s="3"/>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.92927223776240986</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.52663097730093922</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="J40" s="3">
+        <v>0.78162820883950246</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="O40" s="3"/>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.93369237988585629</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0.51237572861077141</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0.76374453810411369</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="O41" s="3"/>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0.93181248713186438</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0.47810807611232747</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="J42" s="3">
+        <v>0.7745329274249132</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O42" s="3"/>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.92872391534372911</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0.49101890834140161</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0.78949950132067181</v>
+      </c>
+      <c r="N43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="O43" s="3"/>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0.93466029419652563</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0.46302753934504709</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0.78153021711246362</v>
+      </c>
+      <c r="N44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="O44" s="3"/>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.92973486428499708</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0.55389486553546741</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="J45" s="3">
+        <v>0.75739746440256905</v>
+      </c>
+      <c r="N45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="O45" s="3"/>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0.92975170256200779</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0.51485494765265138</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="J46" s="3">
+        <v>0.77051436374736282</v>
+      </c>
+      <c r="N46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="O46" s="3"/>
+    </row>
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0.93074855317303662</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0.50449484961317359</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0.7815408127343475</v>
+      </c>
+      <c r="N47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="O47" s="3"/>
+    </row>
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0.93112516016439395</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0.4850380192935817</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="J48" s="3">
+        <v>0.75794159724765886</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="O48" s="3"/>
+    </row>
+    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0.93008155089365496</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0.51056899530882083</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="J49" s="3">
+        <v>0.7767275661938231</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="O49" s="3"/>
+    </row>
+    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0.93086131913458459</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0.52226631985304439</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="J50" s="3">
+        <v>0.78347363738138953</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="O50" s="3"/>
+    </row>
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0.92763428022809524</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0.56792770501704881</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="J51" s="3">
+        <v>0.78451508270848291</v>
+      </c>
+      <c r="N51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="O51" s="3"/>
+    </row>
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0.92863832242031008</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0.52142898800581849</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="J52" s="3">
+        <v>0.7571682834862079</v>
+      </c>
+      <c r="N52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="O52" s="3"/>
+    </row>
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0.92800895050972809</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0.5658557211999734</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="J53" s="3">
+        <v>0.79481763168054775</v>
+      </c>
+      <c r="N53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="O53" s="3"/>
+    </row>
+    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0.93109698007917019</v>
+      </c>
+      <c r="E54" s="3">
+        <v>0.51379303350812111</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J54" s="3">
+        <v>0.77251168034336959</v>
+      </c>
+      <c r="N54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="O54" s="3"/>
+    </row>
+    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="3">
+        <f>AVERAGE(D5:D54)</f>
+        <v>0.93030656165125014</v>
+      </c>
+      <c r="E56" s="3">
+        <f>AVERAGE(E5:E54)</f>
+        <v>0.51291291535470207</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J56" s="3">
+        <f>AVERAGE(J5:J54)</f>
+        <v>0.77549468769363328</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O56" s="3" t="e">
+        <f>AVERAGE(O5:O54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="3">
+        <f>_xlfn.STDEV.S(D5:D54)</f>
+        <v>1.705477609169737E-3</v>
+      </c>
+      <c r="E57" s="3">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>2.4908626127406807E-2</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J57" s="3">
+        <f>_xlfn.STDEV.S(J5:J54)</f>
+        <v>2.4855103371876817E-2</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O57" s="3" t="e">
+        <f>_xlfn.STDEV.S(O5:O54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
@@ -7473,7 +8770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:S65"/>
   <sheetViews>

</xml_diff>